<commit_message>
Update UK coal graphs.
</commit_message>
<xml_diff>
--- a/chapters/ch05-ResourceIntensity/datasets/CoalGraph.xlsx
+++ b/chapters/ch05-ResourceIntensity/datasets/CoalGraph.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/MCBook2021/chapters/ch05-ResourceIntensity/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{D9706CA6-08C3-FE46-9EA5-CE0374445931}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{5A26F381-93DC-2F47-ADD2-95983F3B693B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" tabRatio="629"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" tabRatio="629" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="data to plot" sheetId="4" r:id="rId1"/>
@@ -2527,8 +2527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E262"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A144" workbookViewId="0">
-      <selection activeCell="E183" sqref="E183:E193"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -24081,7 +24081,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E182"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C182"/>
     </sheetView>
   </sheetViews>

</xml_diff>